<commit_message>
--change numbers to strings
</commit_message>
<xml_diff>
--- a/supportTables.xlsx
+++ b/supportTables.xlsx
@@ -3917,7 +3917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3926,6 +3926,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21157,7 +21160,7 @@
   <dimension ref="A1:I803"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="J103" sqref="J103"/>
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23331,7 +23334,7 @@
       <c r="C89">
         <v>0</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="6">
         <v>905</v>
       </c>
       <c r="E89" t="s">
@@ -23357,7 +23360,7 @@
       <c r="C90">
         <v>-1</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="6">
         <v>915</v>
       </c>
       <c r="E90" t="s">
@@ -23383,7 +23386,7 @@
       <c r="C91">
         <v>-2</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="6">
         <v>925</v>
       </c>
       <c r="E91" t="s">
@@ -27612,7 +27615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I801"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A68" workbookViewId="0">
       <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>

</xml_diff>